<commit_message>
updated timesheet with todays hours worked
</commit_message>
<xml_diff>
--- a/Documentation/timesheet.xlsx
+++ b/Documentation/timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="19">
   <si>
     <t>Monday</t>
   </si>
@@ -176,19 +176,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,7 +509,7 @@
   <dimension ref="A2:CA36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AE4" sqref="AE4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,18 +999,114 @@
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AH5" s="3"/>
-      <c r="AL5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="AP5" s="3"/>
       <c r="AT5" s="3"/>
       <c r="AX5" s="3"/>
@@ -1154,48 +1250,48 @@
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13" t="s">
+      <c r="D12" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13" t="s">
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13" t="s">
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13" t="s">
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13" t="s">
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="13"/>
-      <c r="AB12" s="13" t="s">
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="16"/>
+      <c r="AB12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="AC12" s="13"/>
-      <c r="AD12" s="13"/>
-      <c r="AE12" s="13"/>
+      <c r="AC12" s="16"/>
+      <c r="AD12" s="16"/>
+      <c r="AE12" s="16"/>
     </row>
     <row r="13" spans="1:63" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1204,55 +1300,55 @@
       <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="15">
         <f>COUNTIF($C$3:$BK$3, $A13)*0.25</f>
         <v>0.5</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15">
         <f>COUNTIF($C$4:$BK$4, $A13)*0.25</f>
         <v>0</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14">
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15">
         <f>COUNTIF($C$5:$BK$5, $A13)*0.25</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14">
+        <v>1</v>
+      </c>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15">
         <f>COUNTIF($C$6:$BK$6, $A13)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14">
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15">
         <f>COUNTIF($C$7:$BK$7, $A13)*0.25</f>
         <v>0</v>
       </c>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14">
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15">
         <f>COUNTIF($C$8:$BK$8, $A13)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="14">
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15">
         <f>COUNTIF($C$9:$BK$9, $A13)*0.25</f>
         <v>0</v>
       </c>
-      <c r="AC13" s="14"/>
-      <c r="AD13" s="14"/>
-      <c r="AE13" s="14"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="15"/>
     </row>
     <row r="14" spans="1:63" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1261,55 +1357,55 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="15">
         <f>COUNTIF($C$3:$BK$3, $A14)*0.25</f>
         <v>2.25</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14">
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15">
         <f>COUNTIF($C$4:$BK$4, $A14)*0.25</f>
         <v>0.5</v>
       </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14">
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15">
         <f>COUNTIF($C$5:$BK$5, $A14)*0.25</f>
         <v>0</v>
       </c>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14">
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15">
         <f>COUNTIF($C$6:$BK$6, $A14)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14">
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15">
         <f>COUNTIF($C$7:$BK$7, $A14)*0.25</f>
         <v>0</v>
       </c>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14">
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15">
         <f>COUNTIF($C$8:$BK$8, $A14)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="14"/>
-      <c r="AB14" s="14">
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15">
         <f>COUNTIF($C$9:$BK$9, $A14)*0.25</f>
         <v>0</v>
       </c>
-      <c r="AC14" s="14"/>
-      <c r="AD14" s="14"/>
-      <c r="AE14" s="14"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
     </row>
     <row r="15" spans="1:63" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -1318,55 +1414,55 @@
       <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="15">
         <f>COUNTIF($C$3:$BK$3, $A15)*0.25</f>
         <v>8.5</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14">
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15">
         <f>COUNTIF($C$4:$BK$4, $A15)*0.25</f>
         <v>4.5</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14">
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15">
         <f>COUNTIF($C$5:$BK$5, $A15)*0.25</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15">
         <f>COUNTIF($C$6:$BK$6, $A15)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14">
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15">
         <f>COUNTIF($C$7:$BK$7, $A15)*0.25</f>
         <v>0</v>
       </c>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="14"/>
-      <c r="X15" s="14">
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15">
         <f>COUNTIF($C$8:$BK$8, $A15)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="14"/>
-      <c r="AB15" s="14">
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15">
         <f>COUNTIF($C$9:$BK$9, $A15)*0.25</f>
         <v>0</v>
       </c>
-      <c r="AC15" s="14"/>
-      <c r="AD15" s="14"/>
-      <c r="AE15" s="14"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="15"/>
     </row>
     <row r="16" spans="1:63" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1375,183 +1471,183 @@
       <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="15">
         <f>COUNTIF($C$3:$BK$3, $A16)*0.25</f>
         <v>1.5</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14">
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15">
         <f>COUNTIF($C$4:$BK$4, $A16)*0.25</f>
         <v>2</v>
       </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14">
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15">
         <f>COUNTIF($C$5:$BK$5, $A16)*0.25</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14">
+        <v>6.5</v>
+      </c>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15">
         <f>COUNTIF($C$6:$BK$6, $A16)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14">
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15">
         <f>COUNTIF($C$7:$BK$7, $A16)*0.25</f>
         <v>0</v>
       </c>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="14">
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15">
         <f>COUNTIF($C$8:$BK$8, $A16)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="14">
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15">
         <f>COUNTIF($C$9:$BK$9, $A16)*0.25</f>
         <v>0</v>
       </c>
-      <c r="AC16" s="14"/>
-      <c r="AD16" s="14"/>
-      <c r="AE16" s="14"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="15"/>
+      <c r="AE16" s="15"/>
     </row>
     <row r="17" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14">
+      <c r="C17" s="13"/>
+      <c r="D17" s="15">
         <f>COUNTIF($C$3:$BK$3, $A17)*0.25</f>
         <v>2.25</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14">
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15">
         <f>COUNTIF($C$4:$BK$4, $A17)*0.25</f>
         <v>0</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14">
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15">
         <f>COUNTIF($C$5:$BK$5, $A17)*0.25</f>
         <v>0</v>
       </c>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14">
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15">
         <f>COUNTIF($C$6:$BK$6, $A17)*0.25</f>
         <v>0.5</v>
       </c>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14">
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15">
         <f>COUNTIF($C$7:$BK$7, $A17)*0.25</f>
         <v>2</v>
       </c>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="14">
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15">
         <f>COUNTIF($C$8:$BK$8, $A17)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="14">
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15">
         <f>COUNTIF($C$9:$BK$9, $A17)*0.25</f>
         <v>0</v>
       </c>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="14"/>
-      <c r="AE17" s="14"/>
+      <c r="AC17" s="15"/>
+      <c r="AD17" s="15"/>
+      <c r="AE17" s="15"/>
     </row>
     <row r="18" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="D19" s="12">
+      <c r="B19" s="13"/>
+      <c r="D19" s="14">
         <f>D14+D16+D17</f>
         <v>6</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12">
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14">
         <f t="shared" ref="H19" si="0">H14+H16+H17</f>
         <v>2.5</v>
       </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12">
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14">
         <f t="shared" ref="L19" si="1">L14+L16+L17</f>
-        <v>0</v>
-      </c>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12">
+        <v>6.5</v>
+      </c>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14">
         <f t="shared" ref="P19" si="2">P14+P16+P17</f>
         <v>0.5</v>
       </c>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="12"/>
-      <c r="T19" s="12">
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14">
         <f t="shared" ref="T19" si="3">T14+T16+T17</f>
         <v>2</v>
       </c>
-      <c r="U19" s="12"/>
-      <c r="V19" s="12"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="12">
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="14"/>
+      <c r="X19" s="14">
         <f t="shared" ref="X19" si="4">X14+X16+X17</f>
         <v>0</v>
       </c>
-      <c r="Y19" s="12"/>
-      <c r="Z19" s="12"/>
-      <c r="AA19" s="12"/>
-      <c r="AB19" s="12">
+      <c r="Y19" s="14"/>
+      <c r="Z19" s="14"/>
+      <c r="AA19" s="14"/>
+      <c r="AB19" s="14">
         <f t="shared" ref="AB19" si="5">AB14+AB16+AB17</f>
         <v>0</v>
       </c>
-      <c r="AC19" s="12"/>
-      <c r="AD19" s="12"/>
-      <c r="AE19" s="12"/>
-      <c r="AF19" s="12">
+      <c r="AC19" s="14"/>
+      <c r="AD19" s="14"/>
+      <c r="AE19" s="14"/>
+      <c r="AF19" s="14">
         <f>SUM(D19:AE19)</f>
-        <v>11</v>
-      </c>
-      <c r="AG19" s="12"/>
-      <c r="AH19" s="12"/>
-      <c r="AI19" s="12"/>
+        <v>17.5</v>
+      </c>
+      <c r="AG19" s="14"/>
+      <c r="AH19" s="14"/>
+      <c r="AI19" s="14"/>
     </row>
     <row r="20" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
     </row>
     <row r="21" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1571,11 +1667,38 @@
     <row r="36" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="AB15:AE15"/>
+    <mergeCell ref="AF19:AI19"/>
+    <mergeCell ref="AB12:AE12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="T12:W12"/>
+    <mergeCell ref="X12:AA12"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="X13:AA13"/>
+    <mergeCell ref="AB13:AE13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="T14:W14"/>
+    <mergeCell ref="X14:AA14"/>
+    <mergeCell ref="AB14:AE14"/>
+    <mergeCell ref="T13:W13"/>
+    <mergeCell ref="P13:S13"/>
+    <mergeCell ref="T16:W16"/>
+    <mergeCell ref="X16:AA16"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="P15:S15"/>
+    <mergeCell ref="X15:AA15"/>
     <mergeCell ref="AB16:AE16"/>
     <mergeCell ref="T15:W15"/>
     <mergeCell ref="X19:AA19"/>
@@ -1592,38 +1715,11 @@
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="L16:O16"/>
     <mergeCell ref="P16:S16"/>
-    <mergeCell ref="T16:W16"/>
-    <mergeCell ref="X16:AA16"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="P15:S15"/>
-    <mergeCell ref="X13:AA13"/>
-    <mergeCell ref="AB13:AE13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="P14:S14"/>
-    <mergeCell ref="T14:W14"/>
-    <mergeCell ref="X14:AA14"/>
-    <mergeCell ref="AB14:AE14"/>
-    <mergeCell ref="T13:W13"/>
-    <mergeCell ref="X15:AA15"/>
-    <mergeCell ref="AB15:AE15"/>
-    <mergeCell ref="AF19:AI19"/>
-    <mergeCell ref="AB12:AE12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="P12:S12"/>
-    <mergeCell ref="T12:W12"/>
-    <mergeCell ref="X12:AA12"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="P13:S13"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="L19:O19"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:BK9 A13:A19">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">

</xml_diff>

<commit_message>
Modified Speech parser to be more like the final version
</commit_message>
<xml_diff>
--- a/Documentation/timesheet.xlsx
+++ b/Documentation/timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="19">
   <si>
     <t>Monday</t>
   </si>
@@ -175,20 +175,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,7 +509,7 @@
   <dimension ref="A2:CA36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,12 +1129,78 @@
       <c r="F6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AD6" s="3"/>
+      <c r="G6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="AH6" s="3"/>
       <c r="AL6" s="3"/>
       <c r="AP6" s="3"/>
@@ -1250,48 +1316,48 @@
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16" t="s">
+      <c r="D12" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16" t="s">
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16" t="s">
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16" t="s">
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16" t="s">
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="16"/>
-      <c r="AA12" s="16"/>
-      <c r="AB12" s="16" t="s">
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="AC12" s="16"/>
-      <c r="AD12" s="16"/>
-      <c r="AE12" s="16"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="14"/>
+      <c r="AE12" s="14"/>
     </row>
     <row r="13" spans="1:63" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1300,55 +1366,55 @@
       <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <f>COUNTIF($C$3:$BK$3, $A13)*0.25</f>
         <v>0.5</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15">
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12">
         <f>COUNTIF($C$4:$BK$4, $A13)*0.25</f>
         <v>0</v>
       </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15">
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12">
         <f>COUNTIF($C$5:$BK$5, $A13)*0.25</f>
         <v>1</v>
       </c>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15">
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12">
         <f>COUNTIF($C$6:$BK$6, $A13)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15">
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12">
         <f>COUNTIF($C$7:$BK$7, $A13)*0.25</f>
         <v>0</v>
       </c>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15">
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12">
         <f>COUNTIF($C$8:$BK$8, $A13)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="15"/>
-      <c r="AB13" s="15">
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12">
         <f>COUNTIF($C$9:$BK$9, $A13)*0.25</f>
         <v>0</v>
       </c>
-      <c r="AC13" s="15"/>
-      <c r="AD13" s="15"/>
-      <c r="AE13" s="15"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="12"/>
     </row>
     <row r="14" spans="1:63" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1357,55 +1423,55 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <f>COUNTIF($C$3:$BK$3, $A14)*0.25</f>
         <v>2.25</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12">
         <f>COUNTIF($C$4:$BK$4, $A14)*0.25</f>
         <v>0.5</v>
       </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15">
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12">
         <f>COUNTIF($C$5:$BK$5, $A14)*0.25</f>
         <v>0</v>
       </c>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15">
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12">
         <f>COUNTIF($C$6:$BK$6, $A14)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15">
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12">
         <f>COUNTIF($C$7:$BK$7, $A14)*0.25</f>
         <v>0</v>
       </c>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15">
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12">
         <f>COUNTIF($C$8:$BK$8, $A14)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="15">
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="12">
         <f>COUNTIF($C$9:$BK$9, $A14)*0.25</f>
         <v>0</v>
       </c>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="15"/>
+      <c r="AC14" s="12"/>
+      <c r="AD14" s="12"/>
+      <c r="AE14" s="12"/>
     </row>
     <row r="15" spans="1:63" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -1414,55 +1480,55 @@
       <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="12">
         <f>COUNTIF($C$3:$BK$3, $A15)*0.25</f>
         <v>8.5</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15">
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12">
         <f>COUNTIF($C$4:$BK$4, $A15)*0.25</f>
         <v>4.5</v>
       </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15">
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12">
         <f>COUNTIF($C$5:$BK$5, $A15)*0.25</f>
         <v>1.5</v>
       </c>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15">
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12">
         <f>COUNTIF($C$6:$BK$6, $A15)*0.25</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12">
         <f>COUNTIF($C$7:$BK$7, $A15)*0.25</f>
         <v>0</v>
       </c>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15">
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12">
         <f>COUNTIF($C$8:$BK$8, $A15)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="15"/>
-      <c r="AB15" s="15">
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="12">
         <f>COUNTIF($C$9:$BK$9, $A15)*0.25</f>
         <v>0</v>
       </c>
-      <c r="AC15" s="15"/>
-      <c r="AD15" s="15"/>
-      <c r="AE15" s="15"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="12"/>
+      <c r="AE15" s="12"/>
     </row>
     <row r="16" spans="1:63" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1471,183 +1537,183 @@
       <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="12">
         <f>COUNTIF($C$3:$BK$3, $A16)*0.25</f>
         <v>1.5</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12">
         <f>COUNTIF($C$4:$BK$4, $A16)*0.25</f>
         <v>2</v>
       </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15">
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12">
         <f>COUNTIF($C$5:$BK$5, $A16)*0.25</f>
         <v>6.5</v>
       </c>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15">
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12">
         <f>COUNTIF($C$6:$BK$6, $A16)*0.25</f>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12">
         <f>COUNTIF($C$7:$BK$7, $A16)*0.25</f>
         <v>0</v>
       </c>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15">
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12">
         <f>COUNTIF($C$8:$BK$8, $A16)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="15"/>
-      <c r="AB16" s="15">
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12">
         <f>COUNTIF($C$9:$BK$9, $A16)*0.25</f>
         <v>0</v>
       </c>
-      <c r="AC16" s="15"/>
-      <c r="AD16" s="15"/>
-      <c r="AE16" s="15"/>
+      <c r="AC16" s="12"/>
+      <c r="AD16" s="12"/>
+      <c r="AE16" s="12"/>
     </row>
     <row r="17" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="15">
+      <c r="C17" s="15"/>
+      <c r="D17" s="12">
         <f>COUNTIF($C$3:$BK$3, $A17)*0.25</f>
         <v>2.25</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12">
         <f>COUNTIF($C$4:$BK$4, $A17)*0.25</f>
         <v>0</v>
       </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15">
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12">
         <f>COUNTIF($C$5:$BK$5, $A17)*0.25</f>
         <v>0</v>
       </c>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15">
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12">
         <f>COUNTIF($C$6:$BK$6, $A17)*0.25</f>
         <v>0.5</v>
       </c>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15">
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12">
         <f>COUNTIF($C$7:$BK$7, $A17)*0.25</f>
         <v>2</v>
       </c>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15">
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12">
         <f>COUNTIF($C$8:$BK$8, $A17)*0.25</f>
         <v>0</v>
       </c>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-      <c r="AA17" s="15"/>
-      <c r="AB17" s="15">
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="12"/>
+      <c r="AB17" s="12">
         <f>COUNTIF($C$9:$BK$9, $A17)*0.25</f>
         <v>0</v>
       </c>
-      <c r="AC17" s="15"/>
-      <c r="AD17" s="15"/>
-      <c r="AE17" s="15"/>
+      <c r="AC17" s="12"/>
+      <c r="AD17" s="12"/>
+      <c r="AE17" s="12"/>
     </row>
     <row r="18" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="D19" s="14">
+      <c r="B19" s="15"/>
+      <c r="D19" s="13">
         <f>D14+D16+D17</f>
         <v>6</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14">
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13">
         <f t="shared" ref="H19" si="0">H14+H16+H17</f>
         <v>2.5</v>
       </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14">
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13">
         <f t="shared" ref="L19" si="1">L14+L16+L17</f>
         <v>6.5</v>
       </c>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14">
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13">
         <f t="shared" ref="P19" si="2">P14+P16+P17</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13">
         <f t="shared" ref="T19" si="3">T14+T16+T17</f>
         <v>2</v>
       </c>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="14">
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13">
         <f t="shared" ref="X19" si="4">X14+X16+X17</f>
         <v>0</v>
       </c>
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14">
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="13">
         <f t="shared" ref="AB19" si="5">AB14+AB16+AB17</f>
         <v>0</v>
       </c>
-      <c r="AC19" s="14"/>
-      <c r="AD19" s="14"/>
-      <c r="AE19" s="14"/>
-      <c r="AF19" s="14">
+      <c r="AC19" s="13"/>
+      <c r="AD19" s="13"/>
+      <c r="AE19" s="13"/>
+      <c r="AF19" s="13">
         <f>SUM(D19:AE19)</f>
-        <v>17.5</v>
-      </c>
-      <c r="AG19" s="14"/>
-      <c r="AH19" s="14"/>
-      <c r="AI19" s="14"/>
+        <v>21</v>
+      </c>
+      <c r="AG19" s="13"/>
+      <c r="AH19" s="13"/>
+      <c r="AI19" s="13"/>
     </row>
     <row r="20" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
     </row>
     <row r="21" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1667,6 +1733,43 @@
     <row r="36" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="AB16:AE16"/>
+    <mergeCell ref="T15:W15"/>
+    <mergeCell ref="X19:AA19"/>
+    <mergeCell ref="AB19:AE19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="P19:S19"/>
+    <mergeCell ref="T19:W19"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="P17:S17"/>
+    <mergeCell ref="T17:W17"/>
+    <mergeCell ref="X17:AA17"/>
+    <mergeCell ref="AB17:AE17"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="T16:W16"/>
+    <mergeCell ref="X16:AA16"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="P15:S15"/>
+    <mergeCell ref="X15:AA15"/>
+    <mergeCell ref="X13:AA13"/>
+    <mergeCell ref="AB13:AE13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="T14:W14"/>
+    <mergeCell ref="X14:AA14"/>
+    <mergeCell ref="AB14:AE14"/>
+    <mergeCell ref="T13:W13"/>
+    <mergeCell ref="P13:S13"/>
     <mergeCell ref="AB15:AE15"/>
     <mergeCell ref="AF19:AI19"/>
     <mergeCell ref="AB12:AE12"/>
@@ -1683,43 +1786,6 @@
     <mergeCell ref="D17:G17"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="L13:O13"/>
-    <mergeCell ref="X13:AA13"/>
-    <mergeCell ref="AB13:AE13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="P14:S14"/>
-    <mergeCell ref="T14:W14"/>
-    <mergeCell ref="X14:AA14"/>
-    <mergeCell ref="AB14:AE14"/>
-    <mergeCell ref="T13:W13"/>
-    <mergeCell ref="P13:S13"/>
-    <mergeCell ref="T16:W16"/>
-    <mergeCell ref="X16:AA16"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="P15:S15"/>
-    <mergeCell ref="X15:AA15"/>
-    <mergeCell ref="AB16:AE16"/>
-    <mergeCell ref="T15:W15"/>
-    <mergeCell ref="X19:AA19"/>
-    <mergeCell ref="AB19:AE19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="P19:S19"/>
-    <mergeCell ref="T19:W19"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="P17:S17"/>
-    <mergeCell ref="T17:W17"/>
-    <mergeCell ref="X17:AA17"/>
-    <mergeCell ref="AB17:AE17"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="P16:S16"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="L19:O19"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:BK9 A13:A19">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">

</xml_diff>